<commit_message>
cs agent -view DONE
</commit_message>
<xml_diff>
--- a/Data Files/TestData/NexCare/Pengaturan/CS Agent/CS Agent - add.xlsx
+++ b/Data Files/TestData/NexCare/Pengaturan/CS Agent/CS Agent - add.xlsx
@@ -49,13 +49,13 @@
     <t>Cslevel Satu,Cslevel Dua,Cs Officer</t>
   </si>
   <si>
-    <t>November 2022</t>
-  </si>
-  <si>
-    <t>Nov 01 2022</t>
-  </si>
-  <si>
-    <t>Nov 30 2022</t>
+    <t>September 2023</t>
+  </si>
+  <si>
+    <t>Sep 01 2023</t>
+  </si>
+  <si>
+    <t>Sep 30 2023</t>
   </si>
   <si>
     <t>Shift 1</t>
@@ -67,13 +67,13 @@
     <t>Jansen CS,Billy Manasye</t>
   </si>
   <si>
-    <t>September 2022</t>
-  </si>
-  <si>
-    <t>Sep 01 2022</t>
-  </si>
-  <si>
-    <t>Nov 05 2022</t>
+    <t>January 2024</t>
+  </si>
+  <si>
+    <t>Jan 01 2024</t>
+  </si>
+  <si>
+    <t>Jan 15 2024</t>
   </si>
   <si>
     <t>Shift 2</t>
@@ -84,10 +84,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -98,6 +98,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -105,24 +143,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -145,24 +176,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -182,16 +198,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -204,39 +220,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -251,13 +251,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,163 +407,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,6 +442,26 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -484,20 +504,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -517,28 +534,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -547,7 +547,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -556,115 +562,109 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -673,22 +673,22 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1024,7 +1024,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="7"/>
@@ -1108,7 +1108,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>

</xml_diff>